<commit_message>
Option & Book now handle volatility surface: pricing, risk analysis updated. code cleaning: Plots risk cleaned.
</commit_message>
<xml_diff>
--- a/Volatility/Smile.xlsx
+++ b/Volatility/Smile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYTech Student\PycharmProjects\Quantitative_Finance\Volatility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1658D34-08C1-489A-96A3-C6430F021571}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C615935-AE29-444F-94E5-F96B572DE417}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{FC360B08-5FDA-4097-97C1-FD2B012AFD38}"/>
   </bookViews>
@@ -269,19 +269,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.78</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.5</c:v>
@@ -290,16 +290,16 @@
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.56000000000000005</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -385,19 +385,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.75660000000000005</c:v>
+                  <c:v>0.58199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72750000000000004</c:v>
+                  <c:v>0.56259999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67899999999999994</c:v>
+                  <c:v>0.54320000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58199999999999996</c:v>
+                  <c:v>0.52380000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53349999999999997</c:v>
+                  <c:v>0.50439999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.48499999999999999</c:v>
@@ -406,16 +406,16 @@
                   <c:v>0.50439999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.52380000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.54320000000000002</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>0.56259999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.58199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.63049999999999995</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.67899999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,19 +501,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.66300000000000003</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63749999999999996</c:v>
+                  <c:v>0.49299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59499999999999997</c:v>
+                  <c:v>0.47600000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51</c:v>
+                  <c:v>0.45900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46750000000000003</c:v>
+                  <c:v>0.442</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.42499999999999999</c:v>
@@ -522,16 +522,16 @@
                   <c:v>0.442</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.45900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.47600000000000003</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>0.49299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.51</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.55249999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.59499999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -617,19 +617,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.62400000000000011</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60000000000000009</c:v>
+                  <c:v>0.46399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55999999999999994</c:v>
+                  <c:v>0.44800000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48</c:v>
+                  <c:v>0.43200000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44000000000000006</c:v>
+                  <c:v>0.41600000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.4</c:v>
@@ -638,16 +638,16 @@
                   <c:v>0.41600000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.43200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.44800000000000006</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>0.46399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.55999999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,19 +733,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.58499999999999996</c:v>
+                  <c:v>0.44999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.43499999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52499999999999991</c:v>
+                  <c:v>0.42000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.44999999999999996</c:v>
+                  <c:v>0.40500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41250000000000003</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.375</c:v>
@@ -754,16 +754,16 @@
                   <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.40500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.42000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>0.43499999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.44999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.48750000000000004</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.52499999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -851,19 +851,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.56940000000000002</c:v>
+                  <c:v>0.438</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54749999999999999</c:v>
+                  <c:v>0.42339999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51100000000000001</c:v>
+                  <c:v>0.40880000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.438</c:v>
+                  <c:v>0.39419999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.40150000000000002</c:v>
+                  <c:v>0.37959999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.36499999999999999</c:v>
@@ -872,16 +872,16 @@
                   <c:v>0.37959999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.39419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.40880000000000005</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>0.42339999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.438</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.47449999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.51100000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1053,6 +1053,2018 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="140"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:surface3DChart>
+        <c:wireframe val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>day</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="65000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:shade val="65000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ATM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A7FA-4C6E-A747-E412D946FB5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>week</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="82000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="82000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="82000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="82000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:shade val="82000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ATM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.58199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56259999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54320000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52380000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.50439999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50439999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52380000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54320000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56259999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.58199999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A7FA-4C6E-A747-E412D946FB5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>month</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ATM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.49299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A7FA-4C6E-A747-E412D946FB5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>quarter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="83000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="83000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="83000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:tint val="83000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:tint val="83000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ATM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44800000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.44800000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.46399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A7FA-4C6E-A747-E412D946FB5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>half</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:tint val="65000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:tint val="65000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ATM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.44999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43499999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.42000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43499999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A7FA-4C6E-A747-E412D946FB5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="48000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="48000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="48000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:tint val="48000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:tint val="48000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-50%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ATM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.438</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42339999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40880000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.37959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.37959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40880000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42339999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.438</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-A7FA-4C6E-A747-E412D946FB5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:bandFmts>
+          <c:bandFmt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="47000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="47000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="47000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="47000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="47000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="65000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="65000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="65000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="82000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="82000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="82000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="82000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="82000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="83000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="83000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="83000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="83000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="83000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="65000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="65000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="65000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="48000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="48000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="48000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="48000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="48000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="30000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="30000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="30000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="30000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="30000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="8"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="13000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="13000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="13000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="13000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="13000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="9"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="95000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="95000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="95000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="95000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="95000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="10"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="78000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="78000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="78000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="78000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="78000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="11"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="12"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="43000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="43000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="43000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="43000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="43000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="13"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="25000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="25000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="25000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="25000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="25000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="14"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="8000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="8000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="8000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="8000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="8000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+        </c:bandFmts>
+        <c:axId val="1840612543"/>
+        <c:axId val="1719720351"/>
+        <c:axId val="1722556671"/>
+      </c:surface3DChart>
+      <c:catAx>
+        <c:axId val="1840612543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1719720351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1719720351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1840612543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="1722556671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1719720351"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1655,16 +3667,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1684,6 +3696,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>157165</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A316C376-3F98-4F56-9336-898A1EC546C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1992,7 +4040,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,27 +4073,27 @@
         <v>-0.5</v>
       </c>
       <c r="B2" s="2">
-        <v>0.78</v>
+        <v>0.6</v>
       </c>
       <c r="C2" s="2">
         <f>B2*0.97</f>
-        <v>0.75660000000000005</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="D2" s="2">
         <f>B2*0.85</f>
-        <v>0.66300000000000003</v>
+        <v>0.51</v>
       </c>
       <c r="E2" s="2">
         <f>B2*0.8</f>
-        <v>0.62400000000000011</v>
+        <v>0.48</v>
       </c>
       <c r="F2" s="2">
         <f>B2*0.75</f>
-        <v>0.58499999999999996</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="G2" s="2">
         <f>B2*0.73</f>
-        <v>0.56940000000000002</v>
+        <v>0.438</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2053,27 +4101,27 @@
         <v>-0.4</v>
       </c>
       <c r="B3" s="2">
-        <v>0.75</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C12" si="0">B3*0.97</f>
-        <v>0.72750000000000004</v>
+        <v>0.56259999999999999</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D12" si="1">B3*0.85</f>
-        <v>0.63749999999999996</v>
+        <v>0.49299999999999994</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E12" si="2">B3*0.8</f>
-        <v>0.60000000000000009</v>
+        <v>0.46399999999999997</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F12" si="3">B3*0.75</f>
-        <v>0.5625</v>
+        <v>0.43499999999999994</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G12" si="4">B3*0.73</f>
-        <v>0.54749999999999999</v>
+        <v>0.42339999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2081,27 +4129,27 @@
         <v>-0.3</v>
       </c>
       <c r="B4" s="2">
-        <v>0.7</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
-        <v>0.67899999999999994</v>
+        <v>0.54320000000000002</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>0.59499999999999997</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="2"/>
-        <v>0.55999999999999994</v>
+        <v>0.44800000000000006</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="3"/>
-        <v>0.52499999999999991</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="4"/>
-        <v>0.51100000000000001</v>
+        <v>0.40880000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2109,27 +4157,27 @@
         <v>-0.2</v>
       </c>
       <c r="B5" s="2">
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
-        <v>0.58199999999999996</v>
+        <v>0.52380000000000004</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>0.51</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>0.48</v>
+        <v>0.43200000000000005</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="3"/>
-        <v>0.44999999999999996</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="4"/>
-        <v>0.438</v>
+        <v>0.39419999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2137,27 +4185,27 @@
         <v>-0.1</v>
       </c>
       <c r="B6" s="2">
-        <v>0.55000000000000004</v>
+        <v>0.52</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>0.53349999999999997</v>
+        <v>0.50439999999999996</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>0.46750000000000003</v>
+        <v>0.442</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>0.44000000000000006</v>
+        <v>0.41600000000000004</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="3"/>
-        <v>0.41250000000000003</v>
+        <v>0.39</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="4"/>
-        <v>0.40150000000000002</v>
+        <v>0.37959999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2221,27 +4269,27 @@
         <v>0.2</v>
       </c>
       <c r="B9" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.54</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>0.54320000000000002</v>
+        <v>0.52380000000000004</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>0.47600000000000003</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>0.44800000000000006</v>
+        <v>0.43200000000000005</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="3"/>
-        <v>0.42000000000000004</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="4"/>
-        <v>0.40880000000000005</v>
+        <v>0.39419999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2249,27 +4297,27 @@
         <v>0.3</v>
       </c>
       <c r="B10" s="2">
-        <v>0.6</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>0.58199999999999996</v>
+        <v>0.54320000000000002</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>0.51</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>0.48</v>
+        <v>0.44800000000000006</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="3"/>
-        <v>0.44999999999999996</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="4"/>
-        <v>0.438</v>
+        <v>0.40880000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2277,27 +4325,27 @@
         <v>0.4</v>
       </c>
       <c r="B11" s="2">
-        <v>0.65</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>0.63049999999999995</v>
+        <v>0.56259999999999999</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>0.55249999999999999</v>
+        <v>0.49299999999999994</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="2"/>
-        <v>0.52</v>
+        <v>0.46399999999999997</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="3"/>
-        <v>0.48750000000000004</v>
+        <v>0.43499999999999994</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="4"/>
-        <v>0.47449999999999998</v>
+        <v>0.42339999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2305,27 +4353,27 @@
         <v>0.5</v>
       </c>
       <c r="B12" s="2">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>0.67899999999999994</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>0.59499999999999997</v>
+        <v>0.51</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="2"/>
-        <v>0.55999999999999994</v>
+        <v>0.48</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="3"/>
-        <v>0.52499999999999991</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="4"/>
-        <v>0.51100000000000001</v>
+        <v>0.438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>